<commit_message>
Import DS da Phat
Import DS da Phat
</commit_message>
<xml_diff>
--- a/src/views/FileMau/FileMauKhongTuDong.xlsx
+++ b/src/views/FileMau/FileMauKhongTuDong.xlsx
@@ -269,19 +269,19 @@
     <t>13/01/2001</t>
   </si>
   <si>
-    <t>1111</t>
-  </si>
-  <si>
     <t>Nguyễn Việt Trinh</t>
   </si>
   <si>
-    <t>4,2</t>
-  </si>
-  <si>
     <t>5.5</t>
   </si>
   <si>
     <t>HoiDong</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>056201008349</t>
   </si>
 </sst>
 </file>
@@ -780,7 +780,7 @@
   <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +849,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>9</v>
@@ -890,10 +890,10 @@
       <c r="X1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="AA1" s="6" t="s">
@@ -1000,10 +1000,10 @@
       <c r="X2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="Y2" s="11" t="s">
+      <c r="Y2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="Z2" s="9" t="s">
         <v>55</v>
       </c>
       <c r="AA2" s="11" t="s">
@@ -1042,10 +1042,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>66</v>
@@ -1074,7 +1074,7 @@
         <v>71</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="O3" s="22"/>
       <c r="P3" s="22"/>
@@ -1096,7 +1096,7 @@
         <v>5</v>
       </c>
       <c r="Z3" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AA3" s="17">
         <v>6</v>

</xml_diff>